<commit_message>
minor layout and formatting changes
</commit_message>
<xml_diff>
--- a/server/data/resources/KRS15_template.xlsx
+++ b/server/data/resources/KRS15_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Desktop\BMF-DataVis\server\data\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6018F0A6-F57A-43D5-A421-23DF5A6077B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF0B0EC-813F-4F85-AC87-702D75EA3D5D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B728533D-2FCC-42F7-AAD0-D9C231CDF6B6}"/>
+    <workbookView xWindow="14025" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{B728533D-2FCC-42F7-AAD0-D9C231CDF6B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Referenzgroessen" sheetId="1" r:id="rId1"/>
+    <sheet name="KRS15_template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>